<commit_message>
beta test addition of soft reset
beta test
added soft reset function triggered by modbus

also added some comments to the main loop to define each of the 3 modes (standby, setpoint and profile)
</commit_message>
<xml_diff>
--- a/modbus_registers.xlsx
+++ b/modbus_registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\HP_2_Zone_MeltTest_Binaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429E9364-FFC7-4799-9BA5-DFDCD5C01EA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AE7925-62D8-407E-B90D-BA9BB7755EE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="10060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="182">
   <si>
     <t>All Registers:</t>
   </si>
@@ -553,6 +553,24 @@
   </si>
   <si>
     <t>E0</t>
+  </si>
+  <si>
+    <t>    errorstate_reset,               //108</t>
+  </si>
+  <si>
+    <t>,                     //107</t>
+  </si>
+  <si>
+    <t>    soft_reset</t>
+  </si>
+  <si>
+    <t>errorstate_reset</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">used to force the controller to soft reset and ensure a known state </t>
   </si>
 </sst>
 </file>
@@ -928,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3149,10 +3167,37 @@
       </c>
     </row>
     <row r="115" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B115" s="1">
+        <v>107</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="E115" s="1"/>
+      <c r="F115" t="s">
+        <v>116</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B116" s="1">
+        <v>108</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="E116" s="1"/>
+      <c r="F116" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.35">
       <c r="E117" s="1"/>
@@ -3164,9 +3209,15 @@
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C120" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C121" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="2:7" x14ac:dyDescent="0.35">
@@ -3198,6 +3249,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Addition of general purpose inputs
Addition of standby mode monitoring of:
A1 (normally high input with external 10K ohm pullup to 24V)
A2 normally low 24V input
Both go into Modbus for reading with no internal logic or actions
</commit_message>
<xml_diff>
--- a/modbus_registers.xlsx
+++ b/modbus_registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\HP_2_Zone_MeltTest_Binaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3rdWaveLabs\Documents\HP_2_Zone_MeltTest_Binaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AE7925-62D8-407E-B90D-BA9BB7755EE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF734AF-4469-4A66-B14E-6F04F0395FFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="10060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10660" yWindow="670" windowWidth="25200" windowHeight="19030" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="185">
   <si>
     <t>All Registers:</t>
   </si>
@@ -555,12 +555,6 @@
     <t>E0</t>
   </si>
   <si>
-    <t>    errorstate_reset,               //108</t>
-  </si>
-  <si>
-    <t>,                     //107</t>
-  </si>
-  <si>
     <t>    soft_reset</t>
   </si>
   <si>
@@ -571,6 +565,21 @@
   </si>
   <si>
     <t xml:space="preserve">used to force the controller to soft reset and ensure a known state </t>
+  </si>
+  <si>
+    <t>gpi1</t>
+  </si>
+  <si>
+    <t>gpi2</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Maps to A1 as Input with pullup, needs external 10K pullup to 24v due to 24V input circuit, LED A1</t>
+  </si>
+  <si>
+    <t>Maps to Input A2 as standard 24V input (normally low).</t>
   </si>
 </sst>
 </file>
@@ -614,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -628,6 +637,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -946,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3171,17 +3183,17 @@
         <v>107</v>
       </c>
       <c r="C115" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" t="s">
         <v>116</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.35">
@@ -3189,10 +3201,10 @@
         <v>108</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" t="s">
@@ -3200,24 +3212,52 @@
       </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="E117" s="1"/>
+      <c r="B117" s="1">
+        <v>109</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F117" t="s">
+        <v>55</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="E118" s="1"/>
+      <c r="B118" s="1">
+        <v>110</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F118" t="s">
+        <v>55</v>
+      </c>
+      <c r="G118" s="7" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.35">
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C120" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C121" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="2:7" x14ac:dyDescent="0.35">

</xml_diff>